<commit_message>
fixed some stuff, updated excel doc
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_2022_v1.0_EN.xlsx
+++ b/GE3_TestCasesTemplate_2022_v1.0_EN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidatwood/Documents/studyabroad/machinelearningI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30607A4E-D7AD-B249-B873-DEA0CB1E8394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18036BAC-7900-A84B-B3A3-09D4E229DC8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="8240" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1580" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE3 2021 F1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="99">
   <si>
     <t>#</t>
   </si>
@@ -187,6 +187,9 @@
     <t>ID STRING OF LETTERS</t>
   </si>
   <si>
+    <t>ID EMPTY</t>
+  </si>
+  <si>
     <t>"HELLO WORLD"</t>
   </si>
   <si>
@@ -196,12 +199,6 @@
     <t>REG</t>
   </si>
   <si>
-    <t>REGISTRATION_TYPE INVALID</t>
-  </si>
-  <si>
-    <t>ID WITH 36 CHARACTERS?</t>
-  </si>
-  <si>
     <t>REGISTRATION_TYPE EMPTY</t>
   </si>
   <si>
@@ -272,6 +269,75 @@
   </si>
   <si>
     <t>TEST_ECNV3</t>
+  </si>
+  <si>
+    <t>TEST_ECNV4</t>
+  </si>
+  <si>
+    <t>REGISTRATION_TYPE INVALID STRING</t>
+  </si>
+  <si>
+    <t>REGISTRATION_TYPE NOT STRING</t>
+  </si>
+  <si>
+    <t>NAME IS ONLY SPACES</t>
+  </si>
+  <si>
+    <t>"   "</t>
+  </si>
+  <si>
+    <t>TEST_ECNV5</t>
+  </si>
+  <si>
+    <t>TEST_ECNV6</t>
+  </si>
+  <si>
+    <t>TEST_ECNV7</t>
+  </si>
+  <si>
+    <t>TEST_ECNV8</t>
+  </si>
+  <si>
+    <t>TEST_ECNV9</t>
+  </si>
+  <si>
+    <t>TEST_ECNV10</t>
+  </si>
+  <si>
+    <t>TEST_ECNV11</t>
+  </si>
+  <si>
+    <t>TEST_ECNV12</t>
+  </si>
+  <si>
+    <t>2e7ba4f8fc1936352c06a3f200720546</t>
+  </si>
+  <si>
+    <t>VaccineManagementException: "Id received is not a UUID"</t>
+  </si>
+  <si>
+    <t>VaccineManagementException: "Invalid UUID v4 format"</t>
+  </si>
+  <si>
+    <t>VaccineManagementException: "patient_id must be a string value"</t>
+  </si>
+  <si>
+    <t>VaccineManagementException: "registration_type must be either \"REGULAR\" or \"FAMILY\""</t>
+  </si>
+  <si>
+    <t>VaccineManagementException: "registration_type must be a string value"</t>
+  </si>
+  <si>
+    <t>VaccineManagementException: "name_surname must be 30 characters or less"</t>
+  </si>
+  <si>
+    <t>VaccineManagementException: "name_surname must have at least one space"</t>
+  </si>
+  <si>
+    <t>VaccineManagementException: "name_surname may not have leading or trailing spaces"</t>
+  </si>
+  <si>
+    <t>VaccineManagementException: "name_surname must be a string value"</t>
   </si>
 </sst>
 </file>
@@ -288,6 +354,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -436,7 +503,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:O41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:O43">
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="I/O"/>
@@ -689,27 +756,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O998"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="52.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="31.28515625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="17.85546875" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" customWidth="1"/>
-    <col min="14" max="31" width="10.5703125" customWidth="1"/>
+    <col min="14" max="14" width="28.7109375" customWidth="1"/>
+    <col min="15" max="31" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -795,7 +863,9 @@
       <c r="M2" s="1">
         <v>21</v>
       </c>
-      <c r="N2" s="4"/>
+      <c r="N2" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -822,7 +892,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>41</v>
@@ -837,7 +907,7 @@
         <v>21</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="O3" s="4"/>
     </row>
@@ -856,7 +926,7 @@
         <v>39</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>45</v>
@@ -875,7 +945,9 @@
       <c r="M4" s="4">
         <v>21</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -893,7 +965,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>18</v>
@@ -914,7 +986,9 @@
       <c r="M5" s="4">
         <v>21</v>
       </c>
-      <c r="N5" s="4"/>
+      <c r="N5" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -931,13 +1005,15 @@
       <c r="E6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>52</v>
+      <c r="F6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>41</v>
@@ -951,7 +1027,9 @@
       <c r="M6" s="4">
         <v>21</v>
       </c>
-      <c r="N6" s="4"/>
+      <c r="N6" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -968,16 +1046,18 @@
       <c r="E7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>51</v>
+      <c r="F7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="4" t="s">
         <v>40</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>42</v>
@@ -988,48 +1068,49 @@
       <c r="M7" s="4">
         <v>21</v>
       </c>
-      <c r="N7" s="4"/>
+      <c r="N7" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="8" spans="1:15" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="1"/>
+      <c r="F8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="4"/>
       <c r="I8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="4">
-        <v>21</v>
-      </c>
-      <c r="N8" s="4"/>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
+        <f>A8+1</f>
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1037,24 +1118,26 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
-        <v>54</v>
+      <c r="F9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>57</v>
+      <c r="J9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>43</v>
@@ -1062,12 +1145,14 @@
       <c r="M9" s="4">
         <v>21</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <f>A9+1</f>
+        <f t="shared" ref="A10" si="0">A9+1</f>
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1080,9 +1165,11 @@
       <c r="E10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="4" t="s">
@@ -1100,12 +1187,14 @@
       <c r="M10" s="4">
         <v>21</v>
       </c>
-      <c r="N10" s="4"/>
+      <c r="N10" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <f t="shared" ref="A11:A22" si="0">A10+1</f>
+        <f>A10+1</f>
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1118,9 +1207,11 @@
       <c r="E11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="G11" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="4" t="s">
@@ -1129,8 +1220,8 @@
       <c r="J11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K11" s="1">
-        <v>1</v>
+      <c r="K11" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>43</v>
@@ -1138,50 +1229,56 @@
       <c r="M11" s="4">
         <v>21</v>
       </c>
-      <c r="N11" s="4"/>
+      <c r="N11" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A12:A24" si="1">A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="1"/>
+      <c r="F12" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>49</v>
+      <c r="K12" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>43</v>
       </c>
       <c r="M12" s="4">
-        <v>21</v>
-      </c>
-      <c r="N12" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1189,14 +1286,16 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="G13" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="4" t="s">
@@ -1205,21 +1304,23 @@
       <c r="J13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>65</v>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="M13" s="4">
         <v>21</v>
       </c>
-      <c r="N13" s="4"/>
+      <c r="N13" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1227,14 +1328,16 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="G14" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="4" t="s">
@@ -1243,21 +1346,23 @@
       <c r="J14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>42</v>
+      <c r="K14" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="M14" s="4">
         <v>21</v>
       </c>
-      <c r="N14" s="4"/>
+      <c r="N14" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1272,7 +1377,7 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="4" t="s">
@@ -1285,17 +1390,19 @@
         <v>42</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M15" s="4">
         <v>21</v>
       </c>
-      <c r="N15" s="4"/>
+      <c r="N15" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1310,7 +1417,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="4" t="s">
@@ -1322,18 +1429,20 @@
       <c r="K16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>68</v>
+      <c r="L16" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="M16" s="4">
         <v>21</v>
       </c>
-      <c r="N16" s="4"/>
+      <c r="N16" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="O16" s="4"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1348,7 +1457,7 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="4" t="s">
@@ -1361,17 +1470,19 @@
         <v>42</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="M17" s="4">
         <v>21</v>
       </c>
-      <c r="N17" s="4"/>
+      <c r="N17" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="O17" s="4"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1379,14 +1490,14 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>39</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="4" t="s">
@@ -1398,18 +1509,20 @@
       <c r="K18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M18" s="1">
-        <v>5</v>
-      </c>
-      <c r="N18" s="4"/>
+      <c r="L18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M18" s="4">
+        <v>21</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="O18" s="4"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1417,14 +1530,14 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>39</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="4" t="s">
@@ -1436,18 +1549,20 @@
       <c r="K19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M19" s="1">
-        <v>126</v>
-      </c>
-      <c r="N19" s="4"/>
+      <c r="L19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" s="4">
+        <v>21</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="O19" s="4"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1462,7 +1577,7 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="4" t="s">
@@ -1478,14 +1593,16 @@
         <v>43</v>
       </c>
       <c r="M20" s="1">
-        <v>10.01</v>
-      </c>
-      <c r="N20" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="O20" s="4"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1500,7 +1617,7 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="4" t="s">
@@ -1515,15 +1632,17 @@
       <c r="L21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M21" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="N21" s="4"/>
+      <c r="M21" s="1">
+        <v>126</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="O21" s="4"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1537,8 +1656,8 @@
         <v>39</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="5" t="s">
-        <v>74</v>
+      <c r="G22" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="4" t="s">
@@ -1553,44 +1672,92 @@
       <c r="L22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N22" s="4"/>
+      <c r="M22" s="1">
+        <v>10.01</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="O22" s="4"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="4">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="D23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="O23" s="4"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="4">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="D24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="O24" s="4"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1882,8 +2049,40 @@
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+    </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2839,6 +3038,8 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>